<commit_message>
Inclusao custos de transporte no orcamento
</commit_message>
<xml_diff>
--- a/PastaDocsAdministrativos/Orcamento.xlsx
+++ b/PastaDocsAdministrativos/Orcamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logonpflocal\Downloads\GITexercicio\3SIPG-ExemploGit-2024\PastaDocsAdministrativos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42CDF7C-8B0C-4EAA-B0F9-A66588EDF655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CFE5B8-C926-4BBA-BE23-FD746B92E615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>PREVISÃO ORÇAMENTÁRIA - PROJETO EXEMPLO</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>R$ 247.790</t>
+  </si>
+  <si>
+    <t>Transporte</t>
+  </si>
+  <si>
+    <t>R$ 49.780</t>
   </si>
 </sst>
 </file>
@@ -414,7 +420,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,8 +472,12 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>